<commit_message>
level shift test specification created.
</commit_message>
<xml_diff>
--- a/doc/nes-fpga-inter-connect.xlsx
+++ b/doc/nes-fpga-inter-connect.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8490" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8490" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="nes-fpga-interface" sheetId="1" r:id="rId1"/>
     <sheet name="io-pins" sheetId="3" r:id="rId2"/>
     <sheet name="gpio" sheetId="4" r:id="rId3"/>
+    <sheet name="level_shift_test01" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="36">
   <si>
     <t>nes side</t>
   </si>
@@ -97,6 +98,53 @@
   </si>
   <si>
     <t>GND</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>sw</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>led</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>btn</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>inc btn</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rst btn</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>direction</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>gpio 0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>gpio 1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>dir</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>on = cp gpio 0 to 1</t>
+  </si>
+  <si>
+    <t>off = cp gpio 1 to 0</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -3630,6 +3678,2536 @@
         <a:noFill/>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>238124</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>238124</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="正方形/長方形 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="714374" y="2057400"/>
+          <a:ext cx="10715625" cy="3429000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800"/>
+            <a:t>DE0 board</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1800"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="5" name="グループ化 4"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1666875" y="4286250"/>
+          <a:ext cx="238125" cy="514350"/>
+          <a:chOff x="1666875" y="4286250"/>
+          <a:chExt cx="238125" cy="514350"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="正方形/長方形 2"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="514350"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="正方形/長方形 3"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="171450"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="6" name="グループ化 5"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="2143125" y="4286250"/>
+          <a:ext cx="238125" cy="514350"/>
+          <a:chOff x="1666875" y="4286250"/>
+          <a:chExt cx="238125" cy="514350"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="正方形/長方形 6"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="514350"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="正方形/長方形 7"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="171450"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="9" name="グループ化 8"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="2619375" y="4286250"/>
+          <a:ext cx="238125" cy="514350"/>
+          <a:chOff x="1666875" y="4286250"/>
+          <a:chExt cx="238125" cy="514350"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="10" name="正方形/長方形 9"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="514350"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="11" name="正方形/長方形 10"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="171450"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="12" name="グループ化 11"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="3095625" y="4286250"/>
+          <a:ext cx="238125" cy="514350"/>
+          <a:chOff x="1666875" y="4286250"/>
+          <a:chExt cx="238125" cy="514350"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="13" name="正方形/長方形 12"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="514350"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="14" name="正方形/長方形 13"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="171450"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="15" name="グループ化 14"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="3571875" y="4286250"/>
+          <a:ext cx="238125" cy="514350"/>
+          <a:chOff x="1666875" y="4286250"/>
+          <a:chExt cx="238125" cy="514350"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="16" name="正方形/長方形 15"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="514350"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="17" name="正方形/長方形 16"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="171450"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="18" name="グループ化 17"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="4048125" y="4286250"/>
+          <a:ext cx="238125" cy="514350"/>
+          <a:chOff x="1666875" y="4286250"/>
+          <a:chExt cx="238125" cy="514350"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="19" name="正方形/長方形 18"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="514350"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="20" name="正方形/長方形 19"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="171450"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="21" name="グループ化 20"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="4524375" y="4286250"/>
+          <a:ext cx="238125" cy="514350"/>
+          <a:chOff x="1666875" y="4286250"/>
+          <a:chExt cx="238125" cy="514350"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="22" name="正方形/長方形 21"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="514350"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="23" name="正方形/長方形 22"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="171450"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="24" name="グループ化 23"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="5000625" y="4286250"/>
+          <a:ext cx="238125" cy="514350"/>
+          <a:chOff x="1666875" y="4286250"/>
+          <a:chExt cx="238125" cy="514350"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="25" name="正方形/長方形 24"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="514350"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="26" name="正方形/長方形 25"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="171450"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="27" name="グループ化 26"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="5476875" y="4286250"/>
+          <a:ext cx="238125" cy="514350"/>
+          <a:chOff x="1666875" y="4286250"/>
+          <a:chExt cx="238125" cy="514350"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="28" name="正方形/長方形 27"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="514350"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="29" name="正方形/長方形 28"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="171450"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="30" name="グループ化 29"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="5953125" y="4286250"/>
+          <a:ext cx="238125" cy="514350"/>
+          <a:chOff x="1666875" y="4286250"/>
+          <a:chExt cx="238125" cy="514350"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="31" name="正方形/長方形 30"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="514350"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="32" name="正方形/長方形 31"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1666875" y="4286250"/>
+            <a:ext cx="238125" cy="171450"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="正方形/長方形 32"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1666875" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="正方形/長方形 33"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2143125" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="正方形/長方形 34"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2619375" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="正方形/長方形 35"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3095625" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="37" name="正方形/長方形 36"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3571875" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="正方形/長方形 37"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4048125" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="39" name="正方形/長方形 38"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4524375" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="正方形/長方形 39"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5000625" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="41" name="正方形/長方形 40"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5476875" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name="正方形/長方形 41"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5953125" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="45" name="正方形/長方形 44"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7381875" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="46" name="正方形/長方形 45"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3095625" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="47" name="正方形/長方形 46"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3571875" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="正方形/長方形 47"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4048125" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="49" name="正方形/長方形 48"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4524375" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="50" name="正方形/長方形 49"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5000625" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="51" name="正方形/長方形 50"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5476875" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="52" name="正方形/長方形 51"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5953125" y="3771900"/>
+          <a:ext cx="238125" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="53" name="円/楕円 52"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7381875" y="4457700"/>
+          <a:ext cx="476250" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="54" name="円/楕円 53"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8334375" y="4457700"/>
+          <a:ext cx="476250" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="55" name="円/楕円 54"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9286875" y="4457700"/>
+          <a:ext cx="476250" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="56" name="円/楕円 55"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10239375" y="4457700"/>
+          <a:ext cx="476250" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="57" name="正方形/長方形 56"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2505075" y="3600450"/>
+          <a:ext cx="3810000" cy="514350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1800"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="58" name="正方形/長方形 57"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7258050" y="3600450"/>
+          <a:ext cx="3810000" cy="514350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1800"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3890,7 +6468,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4659,7 +7237,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="E3:R44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
@@ -4972,4 +7550,168 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="F20:AT35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="13.5"/>
+  <sheetData>
+    <row r="20" spans="6:46">
+      <c r="L20" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="6:46">
+      <c r="F24" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24">
+        <v>9</v>
+      </c>
+      <c r="J24">
+        <v>8</v>
+      </c>
+      <c r="L24">
+        <v>7</v>
+      </c>
+      <c r="N24">
+        <v>6</v>
+      </c>
+      <c r="P24">
+        <v>5</v>
+      </c>
+      <c r="R24">
+        <v>4</v>
+      </c>
+      <c r="T24">
+        <v>3</v>
+      </c>
+      <c r="V24">
+        <v>2</v>
+      </c>
+      <c r="X24">
+        <v>1</v>
+      </c>
+      <c r="Z24">
+        <v>0</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF24">
+        <v>7</v>
+      </c>
+      <c r="AH24">
+        <v>6</v>
+      </c>
+      <c r="AJ24">
+        <v>5</v>
+      </c>
+      <c r="AL24">
+        <v>4</v>
+      </c>
+      <c r="AN24">
+        <v>3</v>
+      </c>
+      <c r="AP24">
+        <v>2</v>
+      </c>
+      <c r="AR24">
+        <v>1</v>
+      </c>
+      <c r="AT24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="6:46">
+      <c r="F29" t="s">
+        <v>24</v>
+      </c>
+      <c r="H29">
+        <v>9</v>
+      </c>
+      <c r="J29">
+        <v>8</v>
+      </c>
+      <c r="L29">
+        <v>7</v>
+      </c>
+      <c r="N29">
+        <v>6</v>
+      </c>
+      <c r="P29">
+        <v>5</v>
+      </c>
+      <c r="R29">
+        <v>4</v>
+      </c>
+      <c r="T29">
+        <v>3</v>
+      </c>
+      <c r="V29">
+        <v>2</v>
+      </c>
+      <c r="X29">
+        <v>1</v>
+      </c>
+      <c r="Z29">
+        <v>0</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG29">
+        <v>3</v>
+      </c>
+      <c r="AK29">
+        <v>2</v>
+      </c>
+      <c r="AO29">
+        <v>1</v>
+      </c>
+      <c r="AS29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="6:46">
+      <c r="H31" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG31" t="s">
+        <v>27</v>
+      </c>
+      <c r="AS31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="8:9">
+      <c r="H34" t="s">
+        <v>33</v>
+      </c>
+      <c r="I34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="8:9">
+      <c r="H35" t="s">
+        <v>32</v>
+      </c>
+      <c r="I35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
level shifter test fpga logic ok.
</commit_message>
<xml_diff>
--- a/doc/nes-fpga-inter-connect.xlsx
+++ b/doc/nes-fpga-inter-connect.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8490" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8490" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="nes-fpga-interface" sheetId="1" r:id="rId1"/>
@@ -141,10 +141,11 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>on = cp gpio 0 to 1</t>
+    <t>off = cp gpio 1 to 0</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>off = cp gpio 1 to 0</t>
+    <t>on = cp gpio 0 to 1</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -7237,7 +7238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="E3:R44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
@@ -7556,8 +7557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="F20:AT35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="13.5"/>
@@ -7698,7 +7699,7 @@
         <v>33</v>
       </c>
       <c r="I34" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="8:9">
@@ -7706,7 +7707,7 @@
         <v>32</v>
       </c>
       <c r="I35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>